<commit_message>
Matriz de Trazabilidad CU vs Clases finalizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGE/Análisis y Diseño/SGE-MTCC.xlsx
+++ b/Desarrollo/SGE/Análisis y Diseño/SGE-MTCC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabian vargas jimene\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabian vargas jimene\Documents\GitHub\HuayroTech\Desarrollo\SGE\Análisis y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -583,7 +583,7 @@
   <dimension ref="C3:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,18 +754,28 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
@@ -774,18 +784,28 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="7" t="s">
@@ -794,8 +814,12 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
@@ -804,18 +828,28 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
+      <c r="G19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>